<commit_message>
vector weight increase + stock rework
</commit_message>
<xml_diff>
--- a/changes/45-barrels.xlsx
+++ b/changes/45-barrels.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lingl\Documents\deadline-balancing\changes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yifan\Documents\deadline-balancing\changes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AECAFE7C-A445-4EFF-8BCA-5732BD590ECB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B03B5C65-1020-4752-9562-6169F77E81E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="m4-barrels" sheetId="1" r:id="rId1"/>
@@ -92,24 +92,6 @@
     <t>base</t>
   </si>
   <si>
-    <t>ump45_std_200mm_barrel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UMP .45ACP 8" </t>
-  </si>
-  <si>
-    <t>ump45_std_203mm_barrel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UMP .45ACP Threaded 8" </t>
-  </si>
-  <si>
-    <t>ump45_std_420mm_barrel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UMP .45ACP Threaded 16.5" </t>
-  </si>
-  <si>
     <t>vector_45acp_170mm_barrel</t>
   </si>
   <si>
@@ -120,6 +102,24 @@
   </si>
   <si>
     <t>Kriss Vector .45ACP 140mm</t>
+  </si>
+  <si>
+    <t>hk_ump45_200mm_flanged_barrel</t>
+  </si>
+  <si>
+    <t>HK UMP45 200mm .45ACP Flanged</t>
+  </si>
+  <si>
+    <t>hdps_ump45_200mm_threaded_barrel</t>
+  </si>
+  <si>
+    <t>HDPS UMP45 200mm .45ACP Threaded</t>
+  </si>
+  <si>
+    <t>omega_ump45_200mm_trilug_barrel</t>
+  </si>
+  <si>
+    <t>OMEGA UMP45 200mm .45ACP Tri-Lug</t>
   </si>
 </sst>
 </file>
@@ -603,9 +603,8 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -665,9 +664,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -705,7 +704,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -811,7 +810,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -953,7 +952,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -961,76 +960,64 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U38"/>
+  <dimension ref="A1:U22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="27.140625" customWidth="1"/>
+    <col min="1" max="1" width="25.140625" customWidth="1"/>
+    <col min="2" max="2" width="38.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="K2" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="L2" t="s">
         <v>13</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="M2" t="s">
         <v>14</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="N2" t="s">
         <v>3</v>
       </c>
       <c r="P2" t="s">
@@ -1048,44 +1035,41 @@
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3">
-        <v>0.25</v>
+        <v>0.26</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H3">
         <v>0</v>
       </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
       <c r="J3">
-        <v>-38</v>
+        <v>-15</v>
       </c>
       <c r="M3">
         <v>0</v>
       </c>
-      <c r="N3" s="1">
+      <c r="N3">
         <f>C3-D3*20-E3*0.8-F3*0.6-H3*5+I3*10+J3/300</f>
-        <v>-5.1266666666666669</v>
+        <v>-3.05</v>
       </c>
       <c r="P3">
         <v>0.06</v>
       </c>
       <c r="Q3">
-        <v>8</v>
+        <v>7.8740199999999998</v>
       </c>
       <c r="S3">
         <f>ROUND(Q3*0.025+P3+R3, 2)</f>
@@ -1094,44 +1078,41 @@
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C4">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="D4">
-        <v>0.26</v>
+        <v>0.27</v>
       </c>
       <c r="E4">
         <v>1</v>
       </c>
       <c r="F4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H4">
-        <v>0.05</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
+        <v>0.08</v>
       </c>
       <c r="J4">
-        <v>-38</v>
+        <v>-21</v>
       </c>
       <c r="M4">
-        <v>600</v>
-      </c>
-      <c r="N4" s="1">
+        <v>750</v>
+      </c>
+      <c r="N4">
         <f t="shared" ref="N4:N22" si="0">C4-D4*20-E4*0.8-F4*0.6-H4*5+I4*10+J4/300</f>
-        <v>-7.9766666666666666</v>
+        <v>-8.6700000000000017</v>
       </c>
       <c r="P4">
         <v>0.06</v>
       </c>
       <c r="Q4">
-        <v>8</v>
+        <v>7.8740199999999998</v>
       </c>
       <c r="S4">
         <f t="shared" ref="S4:S8" si="1">ROUND(Q4*0.025+P4+R4, 2)</f>
@@ -1140,52 +1121,49 @@
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C5">
-        <v>-4</v>
+        <v>-1</v>
       </c>
       <c r="D5">
-        <v>0.47</v>
+        <v>0.26</v>
       </c>
       <c r="E5">
-        <v>-3</v>
+        <v>0</v>
       </c>
       <c r="F5">
         <v>-2</v>
       </c>
       <c r="H5">
-        <v>-0.1</v>
-      </c>
-      <c r="I5">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="J5">
-        <v>54</v>
+        <v>-18</v>
       </c>
       <c r="M5">
-        <v>1000</v>
-      </c>
-      <c r="N5" s="1">
-        <f t="shared" si="0"/>
-        <v>-8.1199999999999992</v>
+        <v>300</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="0"/>
+        <v>-5.31</v>
       </c>
       <c r="P5">
         <v>0.06</v>
       </c>
       <c r="Q5">
-        <v>16.5</v>
+        <v>7.8740199999999998</v>
       </c>
       <c r="S5">
         <f t="shared" si="1"/>
-        <v>0.47</v>
+        <v>0.26</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="N6" s="1">
+      <c r="N6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1195,44 +1173,42 @@
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" s="1">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7">
         <v>-1</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7">
         <v>0.23</v>
       </c>
-      <c r="E7" s="1">
-        <v>-3</v>
-      </c>
-      <c r="F7" s="1">
-        <v>-3</v>
-      </c>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1">
-        <v>-0.02</v>
-      </c>
-      <c r="I7" s="1">
+      <c r="E7">
+        <v>-1</v>
+      </c>
+      <c r="F7">
+        <v>-1</v>
+      </c>
+      <c r="H7">
+        <v>-0.05</v>
+      </c>
+      <c r="I7">
         <v>0.03</v>
       </c>
-      <c r="J7" s="1">
+      <c r="J7">
         <v>-72</v>
       </c>
-      <c r="K7" s="1">
+      <c r="K7">
         <v>-0.1</v>
       </c>
-      <c r="L7" s="1"/>
-      <c r="M7" s="1">
+      <c r="M7">
         <v>750</v>
       </c>
-      <c r="N7" s="1">
-        <f t="shared" si="0"/>
-        <v>-1.2400000000000002</v>
+      <c r="N7">
+        <f t="shared" si="0"/>
+        <v>-3.8900000000000015</v>
       </c>
       <c r="P7">
         <v>0.06</v>
@@ -1246,44 +1222,42 @@
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" s="1">
-        <v>0</v>
-      </c>
-      <c r="D8" s="1">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
         <v>0.2</v>
       </c>
-      <c r="E8" s="1">
-        <v>-1</v>
-      </c>
-      <c r="F8" s="1">
-        <v>-1</v>
-      </c>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1">
-        <v>0</v>
-      </c>
-      <c r="I8" s="1">
-        <v>0</v>
-      </c>
-      <c r="J8" s="1">
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
         <v>-99</v>
       </c>
-      <c r="K8" s="1">
-        <v>0</v>
-      </c>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1">
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="M8">
         <v>800</v>
       </c>
-      <c r="N8" s="1">
-        <f t="shared" si="0"/>
-        <v>-2.93</v>
+      <c r="N8">
+        <f t="shared" si="0"/>
+        <v>-4.33</v>
       </c>
       <c r="P8">
         <v>0.06</v>
@@ -1297,311 +1271,88 @@
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
-      <c r="N9" s="1">
+      <c r="N9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="1">
+      <c r="N10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
-      <c r="N11" s="1">
+      <c r="N11">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
-      <c r="M12" s="1"/>
-      <c r="N12" s="1">
+      <c r="N12">
         <f>C12-D12*20-E12*0.8-F12*0.6-H12*5+I12*10+J12/300</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
-      <c r="M13" s="1"/>
-      <c r="N13" s="1">
+      <c r="N13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
-      <c r="L14" s="1"/>
-      <c r="M14" s="1"/>
-      <c r="N14" s="1">
+      <c r="N14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
-      <c r="L15" s="1"/>
-      <c r="M15" s="1"/>
-      <c r="N15" s="1">
+      <c r="N15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
-      <c r="M16" s="1"/>
-      <c r="N16" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
-      <c r="M17" s="1"/>
-      <c r="N17" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
-      <c r="L18" s="1"/>
-      <c r="M18" s="1"/>
-      <c r="N18" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="N19" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-      <c r="K20" s="1"/>
-      <c r="L20" s="1"/>
-      <c r="M20" s="1"/>
-      <c r="N20" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-      <c r="K21" s="1"/>
-      <c r="L21" s="1"/>
-      <c r="M21" s="1"/>
-      <c r="N21" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-      <c r="K22" s="1"/>
-      <c r="L22" s="1"/>
-      <c r="M22" s="1"/>
-      <c r="N22" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="N23" s="1"/>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="N24" s="1"/>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="N25" s="1"/>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="N26" s="1"/>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="N27" s="1"/>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="N28" s="1"/>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="N29" s="1"/>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="N30" s="1"/>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="N31" s="1"/>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="N32" s="1"/>
-    </row>
-    <row r="33" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N33" s="1"/>
-    </row>
-    <row r="34" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N34" s="1"/>
-    </row>
-    <row r="35" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N35" s="1"/>
-    </row>
-    <row r="36" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N36" s="1"/>
-    </row>
-    <row r="37" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N37" s="1"/>
-    </row>
-    <row r="38" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N38" s="1"/>
+      <c r="N16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>